<commit_message>
completed demographic data with house values&rent
</commit_message>
<xml_diff>
--- a/data/nh_pop_area.xlsx
+++ b/data/nh_pop_area.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="3860" windowWidth="24760" windowHeight="14340" tabRatio="500"/>
+    <workbookView xWindow="580" yWindow="3860" windowWidth="24760" windowHeight="14340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -1013,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38:E39"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>